<commit_message>
updated cohorts data with information ripped from necropsy files
</commit_message>
<xml_diff>
--- a/cohorts2/raw/NF1 Glioma Mouse Information (Rick).xlsx
+++ b/cohorts2/raw/NF1 Glioma Mouse Information (Rick).xlsx
@@ -33223,8 +33223,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A52921E31622BA47A5BEE7A2CE318F26" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="407fb276827c0378326bfe40beac0cd1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98fb7176-381e-4eb6-825b-93e64c92b6ea" xmlns:ns3="fe56dbcb-f404-42a8-8006-471f9c1a2fc9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4f633fea242de49d6ab069ffd2c9835" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A52921E31622BA47A5BEE7A2CE318F26" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbbe4ce2f8fe09d1c797aa555d1ed32a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98fb7176-381e-4eb6-825b-93e64c92b6ea" xmlns:ns3="fe56dbcb-f404-42a8-8006-471f9c1a2fc9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e562a0e15c5e5c6d0c89a0f84659810" ns2:_="" ns3:_="">
     <xsd:import namespace="98fb7176-381e-4eb6-825b-93e64c92b6ea"/>
     <xsd:import namespace="fe56dbcb-f404-42a8-8006-471f9c1a2fc9"/>
     <xsd:element name="properties">
@@ -33243,6 +33243,7 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -33300,6 +33301,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="19" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -33438,22 +33444,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2C92FBF-B7F5-4497-8D12-D439635B8039}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="98fb7176-381e-4eb6-825b-93e64c92b6ea"/>
-    <ds:schemaRef ds:uri="fe56dbcb-f404-42a8-8006-471f9c1a2fc9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{468B3A14-DF15-4C70-A847-D5FDB65AEC0F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>